<commit_message>
peter's notes - added portability measures; updated first 6 solutions in excel file
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-SolverSolutions.xlsx
+++ b/StateOfPractice/Peter-SolverSolutions.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
   <si>
     <t xml:space="preserve">Sfwr Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Latest Release</t>
+    <t xml:space="preserve">Latest Update Date</t>
   </si>
   <si>
     <t xml:space="preserve">Link</t>
@@ -34,22 +34,205 @@
     <t xml:space="preserve">Academic Sources</t>
   </si>
   <si>
+    <t xml:space="preserve">Latest Citation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computational Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decomposition Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoding of Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception Check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">License</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ouput Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turbulent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complex Geometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Newtonian fluids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependencies</t>
+  </si>
+  <si>
     <t xml:space="preserve">aromanro/LatticeBoltzmann</t>
   </si>
   <si>
+    <t xml:space="preserve">2019 – Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/aromanro/LatticeBoltzmann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blog Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenCL or CUDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atruszkowska/LBM_MATLAB</t>
   </si>
   <si>
+    <t xml:space="preserve">2017 – Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/atruszkowska/LBM_MATLAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shan and Chen multiphase LBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATLAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI</t>
+  </si>
+  <si>
     <t xml:space="preserve">ch4-project</t>
   </si>
   <si>
+    <t xml:space="preserve">2019 – Jul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/SoftwareImpacts/SIMPAC-2019-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eulerian-Lagrangian platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D, 3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C, python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNU GPLv3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDF5, Cmake</t>
+  </si>
+  <si>
     <t xml:space="preserve">CUDA-LBM-simulator</t>
   </si>
   <si>
+    <t xml:space="preserve">2017 – Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/henryfriedlander/CUDA-LBM-simulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPU ACCELERATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nvidia NSight and OpenGL</t>
+  </si>
+  <si>
     <t xml:space="preserve">CudneLB (TCLB)</t>
   </si>
   <si>
+    <t xml:space="preserve">2020 – Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/CFD-GO/TCLB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high-performance CFD simulation code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D 3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q9, D3Q19, D3Q27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI, CUDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nvidia, R, python, </t>
+  </si>
+  <si>
     <t xml:space="preserve">DL_Meso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 – Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scd.stfc.ac.uk/Pages/DL_MESO.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mesoscale simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q9, D3Q15, D3Q19, D3Q27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortran 2003 and C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">academic license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenMP, MPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Development Toolkit,  Paraview and VMD</t>
   </si>
   <si>
     <t xml:space="preserve">ESPResSo</t>
@@ -146,10 +329,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -182,6 +366,20 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -227,7 +425,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,6 +435,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -257,17 +471,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.93"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,65 +498,303 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>53</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>62</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>141</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,7 +802,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +810,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>8</v>
@@ -368,7 +821,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,7 +829,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,7 +837,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>208</v>
@@ -395,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2</v>
@@ -406,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
@@ -417,7 +870,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,7 +886,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,7 +894,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>6</v>
@@ -452,7 +905,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>6</v>
@@ -463,7 +916,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>2</v>
@@ -474,7 +927,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>3</v>
@@ -485,7 +938,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,7 +946,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,7 +954,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,7 +962,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +970,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,7 +978,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,7 +986,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,7 +994,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,7 +1002,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,7 +1010,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,7 +1018,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +1026,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,7 +1034,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,7 +1042,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,7 +1050,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,10 +1058,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://github.com/aromanro/LatticeBoltzmann"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
peter's notes - updated solutions in excel file
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-SolverSolutions.xlsx
+++ b/StateOfPractice/Peter-SolverSolutions.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="221">
   <si>
     <t xml:space="preserve">Sfwr Name</t>
   </si>
@@ -37,7 +38,7 @@
     <t xml:space="preserve">Latest Citation</t>
   </si>
   <si>
-    <t xml:space="preserve">Category</t>
+    <t xml:space="preserve">Category Notes</t>
   </si>
   <si>
     <t xml:space="preserve">Dimensions</t>
@@ -238,91 +239,451 @@
     <t xml:space="preserve">ESPResSo</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/espressomd/espresso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular Dynamics many-particle simulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3Q19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++, Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmake, Boost, FFTW, Python, Cython </t>
+  </si>
+  <si>
     <t xml:space="preserve">ESPResSo++</t>
   </si>
   <si>
+    <t xml:space="preserve">2019 – Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/espressopp/espressopp/releases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grained atomistic or bead-spring models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python, Numpy</t>
+  </si>
+  <si>
     <t xml:space="preserve">firesim</t>
   </si>
   <si>
+    <t xml:space="preserve">2014 – Jan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/kynan/firesim/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachelor Thesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmake, Boost, Irrlicht</t>
+  </si>
+  <si>
     <t xml:space="preserve">fvLBM</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/zhulianhua/fvLBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unfinished finite volume LBM solver</t>
+  </si>
+  <si>
     <t xml:space="preserve">HemeLB</t>
   </si>
   <si>
-    <t xml:space="preserve">JavaCFD</t>
+    <t xml:space="preserve">2018 – Aug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/UCL/hemelb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemodynamics in sparse geometries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmake</t>
   </si>
   <si>
     <t xml:space="preserve">JFlowSim</t>
   </si>
   <si>
+    <t xml:space="preserve">2017 – Dec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/ChristianFJanssen/jflowsim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thread-parallel Lattice Boltzmann CFD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java</t>
+  </si>
+  <si>
     <t xml:space="preserve">laboetie</t>
   </si>
   <si>
+    <t xml:space="preserve">2018 – Aug </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/maxlevesque/laboetie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chemical application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortran 90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNU GPLv2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenMP</t>
+  </si>
+  <si>
     <t xml:space="preserve">LatBo.jl</t>
   </si>
   <si>
+    <t xml:space="preserve">2017 – Feb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/UCL/LatBo.jl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q9, D3Q19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIT "Expat"</t>
+  </si>
+  <si>
     <t xml:space="preserve">lettuce</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/Olllom/lettuce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBM based on PyTorch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIT license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUDA, MPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conda, Python</t>
+  </si>
+  <si>
     <t xml:space="preserve">LB2D_Prime</t>
   </si>
   <si>
+    <t xml:space="preserve">http://faculty.fiu.edu/~sukopm/LBnD_Prime/LBnD_Prime.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complementary to the text “LatticeBoltzmannModeling”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORTRAN90, Python, C</t>
+  </si>
+  <si>
     <t xml:space="preserve">LB3D</t>
   </si>
   <si>
+    <t xml:space="preserve">http://ccs.chem.ucl.ac.uk/lb3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shan-Chen model for binary fluid interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORTRAN 90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGPL version 3.</t>
+  </si>
+  <si>
     <t xml:space="preserve">LBDEMcoupling-public</t>
   </si>
   <si>
+    <t xml:space="preserve">2017 – Jan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/ParticulateFlow/LBDEMcoupling-public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling between the Lattice-Boltzmann code Palabos and the DEM code LIGGGHTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPLv3</t>
+  </si>
+  <si>
     <t xml:space="preserve">LBSim</t>
   </si>
   <si>
+    <t xml:space="preserve">2015 – Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/noirb/lbsim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supporting complex boundaries</t>
+  </si>
+  <si>
     <t xml:space="preserve">Limbes</t>
   </si>
   <si>
+    <t xml:space="preserve">https://code.google.com/archive/p/limbes/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">academic numerical tool `easy to use' based on kinetic models for typical situations encountered in microfluidics/ Gauss-Hermite quadrature</t>
+  </si>
+  <si>
     <t xml:space="preserve">listLBM</t>
   </si>
   <si>
+    <t xml:space="preserve">2017 – Nov </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/sorush-khajepor/listLBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhD / porous media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortran 2003 and 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmake, VDKFortran</t>
+  </si>
+  <si>
     <t xml:space="preserve">LUMA</t>
   </si>
   <si>
+    <t xml:space="preserve">2018 – Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/ElsevierSoftwareX/SOFTX-D-18-00007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fluid structure interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C, C++</t>
+  </si>
+  <si>
     <t xml:space="preserve">MP-LABS</t>
   </si>
   <si>
+    <t xml:space="preserve">2014 – Oct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/carlosrosales/mplabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiphase Lattice Boltzmann Suite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI, OpenMP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Openlb</t>
   </si>
   <si>
+    <t xml:space="preserve">2019 – Sept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.openlb.net/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">library for LB simulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q5, D2Q9, D3Q7, D3Q13, D3Q15, D3Q19, D3Q27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNU GPL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palabos</t>
   </si>
   <si>
+    <t xml:space="preserve">2019 – Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://palabos.unige.ch/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFD solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q9, D3Q13, D3Q15, D3Q19, D3Q27.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNU APGLV3</t>
+  </si>
+  <si>
     <t xml:space="preserve">pyLBM</t>
   </si>
   <si>
+    <t xml:space="preserve">2020 – Jan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/pylbm/pylbm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all in one package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1D, 2D, 3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1Q2, D1Q3, D2Q5, D2Q9, DQ15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSD License</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cython, NumPy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sailfish</t>
   </si>
   <si>
+    <t xml:space="preserve">2019 – Nov </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/sailfish-team/sailfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulation package for GPUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGPL v3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUDA, OpenCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numpy-1.7.0 scipy-0.13.0 sympy-0.7.3 mako-0.9.0 execnet-1.0.9 pyzmq-14.0.0 netifaces-0.8 (for distributed simulations only) a Python module for the computational backend ,      pygame     matplotlib     wxpython , matplotlib</t>
+  </si>
+  <si>
     <t xml:space="preserve">siramirsaman/LBM</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/siramirsaman/LBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curved Boundaries </t>
+  </si>
+  <si>
     <t xml:space="preserve">SunlightLB</t>
   </si>
   <si>
+    <t xml:space="preserve">2012 – Dec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://sunlightlb.sourceforge.net/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrodynamics problems, including passive scalar transport problems</t>
+  </si>
+  <si>
     <t xml:space="preserve">Taxila-LBM</t>
   </si>
   <si>
+    <t xml:space="preserve">2017 – Jun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/ecoon/Taxila-LBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lattice Boltzmann code from LANL , Shan and Chen Lattice Boltzmann Method </t>
+  </si>
+  <si>
     <t xml:space="preserve">loliverhennigh</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/loliverhennigh/Lattice-Boltzmann-fluid-flow-in-Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">written in Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q5, D3Q15, D3Q19</t>
+  </si>
+  <si>
     <t xml:space="preserve">turbulent_lbm_multigpu</t>
   </si>
   <si>
+    <t xml:space="preserve">2014 – Feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/arashb/turbulent_lbm_multigpu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turbulent fluid flow on GPU Cluster </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apache License, Version 2.0 </t>
+  </si>
+  <si>
     <t xml:space="preserve">waLBerla</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.walberla.net/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">massively parallel framework for multi physics applications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2Q5, D2Q9, D3Q15, D3Q19, D3Q27 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI, Boost</t>
+  </si>
+  <si>
     <t xml:space="preserve">wlb</t>
   </si>
   <si>
+    <t xml:space="preserve">2013 – Jun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/weierstrass/wlb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coupled equations in electrohydrodynamics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1D, 2D</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zmhhaha/LBM-Cplusplus-A.A.Mohamad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020 – Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/zmhhaha/LBM-Cplusplus-A.A.Mohamad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lattice Boltzmann Method Fundamentals and Engineering Applications with Computer Codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++ </t>
   </si>
 </sst>
 </file>
@@ -471,13 +832,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ37"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ36"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S35" activeCellId="0" sqref="S35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
@@ -797,31 +1181,118 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -829,40 +1300,133 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>208</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
+        <v>101</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>103</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="V14" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +1434,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>108</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,59 +1469,197 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="V16" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>125</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>142</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>82</v>
+        <v>130</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>83</v>
+        <v>135</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>137</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>139</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>140</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +1667,40 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>142</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="O22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,15 +1708,72 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>87</v>
+        <v>154</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="V24" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -962,103 +1781,407 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>159</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>672</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>171</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="V27" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>179</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="V28" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>186</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>189</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>193</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="O31" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O33" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>206</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="O34" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="V34" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>211</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>100</v>
+        <v>216</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="N36" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>